<commit_message>
Importar e classificar finalizado
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="220">
   <si>
     <t>Índice</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Classificação</t>
   </si>
   <si>
-    <t>Texto</t>
+    <t>Sugestão</t>
   </si>
   <si>
     <t>2024-06</t>
@@ -636,589 +636,40 @@
     <t>Receita</t>
   </si>
   <si>
-    <t>Revisão Manual</t>
-  </si>
-  <si>
-    <t>Muai Thay</t>
+    <t>Onibus</t>
+  </si>
+  <si>
+    <t>Viajem</t>
+  </si>
+  <si>
+    <t>Maui Thay</t>
+  </si>
+  <si>
+    <t>Presente</t>
+  </si>
+  <si>
+    <t>Avião</t>
   </si>
   <si>
     <t>Roupas</t>
   </si>
   <si>
+    <t>Perfume</t>
+  </si>
+  <si>
+    <t>Utrnsílios</t>
+  </si>
+  <si>
+    <t>Lanche</t>
+  </si>
+  <si>
     <t>Streaming</t>
   </si>
   <si>
-    <t>Wemobi - Parcela 3/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Bikeprosports - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Clicktrip*Clicktrip - Parcela 1/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Latam Airlin*Nomyxq018 - Parcela 4/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Jucilene da Silva - Parcela 2/6 Muai Thay</t>
-  </si>
-  <si>
-    <t>Amazon Marketplace - Parcela 4/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Wemobi - Parcela 2/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Wemobi - Mobilidade e - Parcela 3/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag Eucatur*Eucatur - Parcela 3/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Gol Linhas A*Mysxqi010 - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pagamento recebido Sem Classificação</t>
-  </si>
-  <si>
-    <t>Via Brasil Continente - Parcela 1/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Decathlon Floripa Cont Roupas</t>
-  </si>
-  <si>
-    <t>Hna*Oboticario - Parcela 1/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Mercadolivre*Mercadol - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Saldo restante da fatura anterior Sem Classificação</t>
-  </si>
-  <si>
-    <t>Decathlon Paulista - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Google Storage Sem Classificação</t>
-  </si>
-  <si>
-    <t>Netflix Entretenimento Streaming</t>
-  </si>
-  <si>
-    <t>Dm*Helpmaxcom Streaming</t>
-  </si>
-  <si>
-    <t>Pagamento de boleto efetuado - FUNDACAO CELESC DE SEGURIDADE SOCIAL Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência recebida pelo Pix - RODRIK J S M ARAUJO SOUSA - •••.204.832-•• - BCO DO BRASIL S.A. (0001) Agência: 2290 Conta: 76490-6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência recebida pelo Pix - ROZANI ELIZABET SCHAU MENEZES - •••.976.190-•• - ITAÚ UNIBANCO S.A. (0341) Agência: 4730 Conta: 14906-1 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pagamento de fatura Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Roodger Nathanael Schau Menezes Araujo de Sousa - •••.204.912-•• - Nubank (0260) Agência: 1 Conta: 33833840-6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Solimar Pereira dos Santos de Arruda Pinto - •••.656.441-•• - BCO SANTANDER (BRASIL) S.A. (0033) Agência: 3131 Conta: 2011547-4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Diandra Brasil - •••.339.669-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 1354143-2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Camila Pizzetti Dal Toe - •••.804.129-•• - CAIXA ECONOMICA FEDERAL (0104) Agência: 1011 Conta: 3701000000590663719-9 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Celina Selister Martins - •••.045.580-•• - Nubank (0260) Agência: 1 Conta: 71403468-4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência Recebida - Caroline Ferreira Roberto - •••.574.268-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 8831014-4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Resgate RDB Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Dunas Burguer Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Shopee - 38.372.267/0001-82 - ADYEN DO BRASIL IP LTDA. Agência: 1 Conta: 100000037-5 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mokka Emporium Sem Classificação</t>
-  </si>
-  <si>
-    <t>Hna*Oboticario - Parcela 2/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Jucilene da Silva - Parcela 3/6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Mercadolivre*Mercadol - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Decathlon Paulista - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Via Brasil Continente - Parcela 2/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Clicktrip*Clicktrip - Parcela 2/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag*Principiaes Sem Classificação</t>
-  </si>
-  <si>
-    <t>Aliexpress - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Raia3429 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Dunas Burguer Sem Classificação</t>
-  </si>
-  <si>
-    <t>Mba Usp Esalq Sem Classificação</t>
-  </si>
-  <si>
-    <t>Hna*Oboticario - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Itaguacu Administrado Sem Classificação</t>
-  </si>
-  <si>
-    <t>Niko Sushi Bar Sem Classificação</t>
-  </si>
-  <si>
-    <t>Estrela Poke Sushi Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag*Pensanoevento Sem Classificação</t>
-  </si>
-  <si>
-    <t>Kibelandia Sem Classificação</t>
-  </si>
-  <si>
-    <t>Merci Downtown Sem Classificação</t>
-  </si>
-  <si>
-    <t>Boteco Sem Classificação</t>
-  </si>
-  <si>
-    <t>Estorno de "Pag*Pensanoevento" Sem Classificação</t>
-  </si>
-  <si>
-    <t>Restaurante Antenas Sem Classificação</t>
-  </si>
-  <si>
-    <t>Netflix.Com Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag*Parrilenha Sem Classificação</t>
-  </si>
-  <si>
-    <t>Meu Jardim Food Park Sem Classificação</t>
-  </si>
-  <si>
-    <t>Dm*Helpmaxcom Sem Classificação</t>
-  </si>
-  <si>
-    <t>Ebn *Sonyplaystatn Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pagamento de boleto efetuado - EMPRESA DE PESQUISA ENERGETICA - EPE / 8  Con Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Don Floripa Food And A Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Smart Consultoria Sem Classificação</t>
-  </si>
-  <si>
-    <t>Aplicação - Tesouro IPCA+ 2029 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - ROZANI ELIZABET SCHAU MENEZES - •••.976.190-•• - ITAÚ UNIBANCO S.A. (0341) Agência: 4730 Conta: 14906-1 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Ana Paula Klaumann - •••.959.609-•• - BCO DO BRASIL S.A. (0001) Agência: 1453 Conta: 60976-5 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Aplicação RDB Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Raia3429 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Continente Park Sao Jo Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Swell Poke Sj Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Chq Floripa Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Continente Shopping Es Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mu Msj Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Uma Origem Cafe Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Uncle Joes Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Restaurante Vo Maneca Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Pag*Ronivondeoliveira Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Ppn Comercio Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Pag*Pasteisdabarra Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Tamar Sul Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Pag*Patriciaberta Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - ANDRESSA RAMOS SIQUEIRA SILVA - •••.209.918-•• - BCO DO BRASIL S.A. (0001) Agência: 1453 Conta: 86145-6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Barbeariarany Sem Classificação</t>
-  </si>
-  <si>
-    <t>Clicktrip*Clicktrip - Parcela 3/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Hna*Oboticario - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Via Brasil Continente - Parcela 3/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Panvel Farmacias Sem Classificação</t>
-  </si>
-  <si>
-    <t>Jucilene da Silva - Parcela 4/6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Hna*Oboticario - Parcela 3/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Aliexpress - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pg *Ton Very Pizza Sem Classificação</t>
-  </si>
-  <si>
-    <t>Mp *Ingressos690 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Silva Kosinski Pizzar Sem Classificação</t>
-  </si>
-  <si>
-    <t>Wemobi - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag*Alamirritamaria Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag*Kebabfaruk Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pit Floripa Smoked Hou Sem Classificação</t>
-  </si>
-  <si>
-    <t>Google One Sem Classificação</t>
-  </si>
-  <si>
-    <t>Spitfire Pizza Lagoa Sem Classificação</t>
-  </si>
-  <si>
-    <t>Liffey Sem Classificação</t>
-  </si>
-  <si>
-    <t>Tamar Sul Sem Classificação</t>
-  </si>
-  <si>
-    <t>Cafe Pacai Sem Classificação</t>
-  </si>
-  <si>
-    <t>App*Barbeariaon1210 - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Pag*Welovesushi Sem Classificação</t>
-  </si>
-  <si>
-    <t>Azul We*Vhuqvssousa - Parcela 1/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Spitfire Pizza Lagoa Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - 46193392 Lucas Merino Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Floripao Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Zp*Ifoodqushdoc8565b0 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - O Tao Delivery Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Consagrado Burger Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Carolina da Cruz Carneiro - •••.890.392-•• - BANCO INTER (0077) Agência: 1 Conta: 6800727-2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Aplicação - Tesouro Selic 2029 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Ghazalarabianfood Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Nefasta Cervejaria Art Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Multipark Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Posto Brasol Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Chilli Willy Cozinha M Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Snack Bar Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Multipark Assembleia Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Logbank*Cervejaria Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Hello Donuts Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Pagarme Pagamentos SA - 18.727.053/0001-74 - STONE IP S.A. (0197) Agência: 1 Conta: 16714636-4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mcandomilfarias Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Bertol Craft Beer Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Posto Vila Rica Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Vitamar Comercio de C Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Cb Florianopolis Comer Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Funcional Suplemento Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Merci Downtown Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mana Poke Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Gaafer Chocolateria Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Somacoworking Sem Classificação</t>
-  </si>
-  <si>
-    <t>App*Barbeariaon1210 - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Jucilene da Silva - Parcela 5/6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Clicktrip*Clicktrip - Parcela 4/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Wemobi - Parcela 2/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Azul We*Vhuqvssousa - Parcela 2/4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Amazon - Parcela 1/3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Uber *Uber *Trip Sem Classificação</t>
-  </si>
-  <si>
-    <t>Hai Poke Sem Classificação</t>
-  </si>
-  <si>
-    <t>Mp *Gamplay Sem Classificação</t>
-  </si>
-  <si>
-    <t>Gelatony Sem Classificação</t>
-  </si>
-  <si>
-    <t>Ifd*Bdg Delivery de Al Sem Classificação</t>
-  </si>
-  <si>
-    <t>Shopee *Jrbeleza Sem Classificação</t>
-  </si>
-  <si>
-    <t>Wemobi - Mobilidade e - Parcela 1/2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Brukar Oficina Sem Classificação</t>
-  </si>
-  <si>
-    <t>Netflix Entretenimento Sem Classificação</t>
-  </si>
-  <si>
-    <t>Natura Pay*Atn - B3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Lupi Comercio de Alime Sem Classificação</t>
-  </si>
-  <si>
-    <t>Gelateria Freddo Sem Classificação</t>
-  </si>
-  <si>
-    <t>Estimada Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Abdelazizbahsain Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - 53257497 Marceli Marqu Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Niko Sushi Bar Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência recebida pelo Pix - RODRIGO FERNANDO OLIVEIRA CABECA NEVES - •••.416.542-•• - BCO BRADESCO S.A. (0237) Agência: 2398 Conta: 20884-1 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Koxixos Beer Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mp *Mrsmoketabaca Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Komtodos Restaurante Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Milium Loja Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Subway Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Bulebarcafe Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Suru Bar Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - JAIRO CORTES FERREIRA - •••.476.297-•• - PICPAY (0380) Agência: 1 Conta: 89129718-9 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mane Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Triba'S Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Toca da Lapa Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Toca da Lapa Bar Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Mp *Keity Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Caroline Ferreira Roberto - •••.574.268-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 8831014-4 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Auttar Loja Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Casa das Iguarias Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Imperio Tres Comercio Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Rodrik Jose Schau Menezes Araujo de Sousa - •••.204.832-•• - BANCO BTG PACTUAL S.A. (0208) Agência: 1 Conta: 257923-3 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Supermercados Angeloni Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada - RODRIK JOSE SCHAU MENEZES ARAUJO DE SOUSA - •••.204.832-•• - XP Investimentos Corretora de Câmbio Títulos e Valores Mobiliários S.A. (0102) Agência: 2 Conta: 272575-9 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Antonio Marcos Machado - •••.647.269-•• - BCO DO BRASIL S.A. (0001) Agência: 1453 Conta: 50252-9 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Leonardo Camargo Momm - •••.465.239-•• - BCO DO BRASIL S.A. (0001) Agência: 5201 Conta: 1586753-6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - Rohannah Ster Schau Menezes Araújo de Sousa - •••.205.052-•• - Nubank (0260) Agência: 1 Conta: 9128823-6 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Hpl2alimentosltda Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Super Imperatriz Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Poke Flow Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Posto Capoeiras Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - COMMERCEGATE BRASIL PAGAMENTOS E TECNOLOGIA - 45.651.293/0001-05 - IUGU IP S.A. (0401) Agência: 2 Conta: 220778-2 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - EMERSON EDSON DOS SANTOS DE AZEVEDO - •••.832.579-•• - BCO C6 S.A. (0336) Agência: 1 Conta: 18719897-7 Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Berlinf*Parada do Japo Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Wfphones Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Rodosnack Petropen Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Zp*Restaurante Serra D Sem Classificação</t>
-  </si>
-  <si>
-    <t>Compra no débito - Camilleferreira Sem Classificação</t>
-  </si>
-  <si>
-    <t>Transferência enviada pelo Pix - SIM.DIGITAL - 29.911.764/0001-10 - CCLA MAXI ALFA Agência: 3069 Conta: 175502-1 Sem Classificação</t>
+    <t>Salário</t>
+  </si>
+  <si>
+    <t>Invesimento</t>
   </si>
   <si>
     <t>Frequência</t>
@@ -1649,8 +1100,8 @@
       <c r="H2" t="s">
         <v>206</v>
       </c>
-      <c r="I2" t="s">
-        <v>210</v>
+      <c r="I2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1678,8 +1129,8 @@
       <c r="H3" t="s">
         <v>206</v>
       </c>
-      <c r="I3" t="s">
-        <v>211</v>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1705,10 +1156,10 @@
         <v>71.72</v>
       </c>
       <c r="H4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1736,8 +1187,8 @@
       <c r="H5" t="s">
         <v>206</v>
       </c>
-      <c r="I5" t="s">
-        <v>213</v>
+      <c r="I5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1763,10 +1214,10 @@
         <v>120</v>
       </c>
       <c r="H6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I6" t="s">
-        <v>214</v>
+        <v>208</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1794,8 +1245,8 @@
       <c r="H7" t="s">
         <v>206</v>
       </c>
-      <c r="I7" t="s">
-        <v>210</v>
+      <c r="I7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1823,8 +1274,8 @@
       <c r="H8" t="s">
         <v>206</v>
       </c>
-      <c r="I8" t="s">
-        <v>210</v>
+      <c r="I8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1850,10 +1301,10 @@
         <v>53.07</v>
       </c>
       <c r="H9" t="s">
-        <v>206</v>
-      </c>
-      <c r="I9" t="s">
-        <v>215</v>
+        <v>209</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1881,8 +1332,8 @@
       <c r="H10" t="s">
         <v>206</v>
       </c>
-      <c r="I10" t="s">
-        <v>216</v>
+      <c r="I10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1910,8 +1361,8 @@
       <c r="H11" t="s">
         <v>206</v>
       </c>
-      <c r="I11" t="s">
-        <v>217</v>
+      <c r="I11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1939,8 +1390,8 @@
       <c r="H12" t="s">
         <v>206</v>
       </c>
-      <c r="I12" t="s">
-        <v>218</v>
+      <c r="I12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1966,10 +1417,10 @@
         <v>137.05</v>
       </c>
       <c r="H13" t="s">
-        <v>206</v>
-      </c>
-      <c r="I13" t="s">
-        <v>219</v>
+        <v>210</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1995,10 +1446,10 @@
         <v>1657.81</v>
       </c>
       <c r="H14" t="s">
-        <v>206</v>
-      </c>
-      <c r="I14" t="s">
-        <v>220</v>
+        <v>205</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2024,10 +1475,10 @@
         <v>46.66</v>
       </c>
       <c r="H15" t="s">
-        <v>206</v>
-      </c>
-      <c r="I15" t="s">
-        <v>221</v>
+        <v>209</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2053,10 +1504,10 @@
         <v>69.98</v>
       </c>
       <c r="H16" t="s">
-        <v>208</v>
-      </c>
-      <c r="I16" t="s">
-        <v>222</v>
+        <v>211</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2082,10 +1533,10 @@
         <v>118.49</v>
       </c>
       <c r="H17" t="s">
-        <v>206</v>
-      </c>
-      <c r="I17" t="s">
-        <v>223</v>
+        <v>212</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2111,10 +1562,10 @@
         <v>24.5</v>
       </c>
       <c r="H18" t="s">
-        <v>206</v>
-      </c>
-      <c r="I18" t="s">
-        <v>224</v>
+        <v>213</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2140,10 +1591,10 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>206</v>
-      </c>
-      <c r="I19" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2169,10 +1620,10 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>206</v>
-      </c>
-      <c r="I20" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2198,10 +1649,10 @@
         <v>88.5</v>
       </c>
       <c r="H21" t="s">
-        <v>206</v>
-      </c>
-      <c r="I21" t="s">
-        <v>226</v>
+        <v>211</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2227,10 +1678,10 @@
         <v>7.99</v>
       </c>
       <c r="H22" t="s">
-        <v>206</v>
-      </c>
-      <c r="I22" t="s">
-        <v>227</v>
+        <v>214</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2256,10 +1707,10 @@
         <v>18.9</v>
       </c>
       <c r="H23" t="s">
-        <v>209</v>
-      </c>
-      <c r="I23" t="s">
-        <v>228</v>
+        <v>215</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2285,10 +1736,10 @@
         <v>17.45</v>
       </c>
       <c r="H24" t="s">
-        <v>209</v>
-      </c>
-      <c r="I24" t="s">
-        <v>229</v>
+        <v>215</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2314,10 +1765,10 @@
         <v>449.82</v>
       </c>
       <c r="H25" t="s">
-        <v>206</v>
-      </c>
-      <c r="I25" t="s">
-        <v>230</v>
+        <v>205</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2343,10 +1794,10 @@
         <v>2000</v>
       </c>
       <c r="H26" t="s">
-        <v>206</v>
-      </c>
-      <c r="I26" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2372,10 +1823,10 @@
         <v>191.66</v>
       </c>
       <c r="H27" t="s">
-        <v>206</v>
-      </c>
-      <c r="I27" t="s">
-        <v>232</v>
+        <v>216</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2401,10 +1852,10 @@
         <v>368.41</v>
       </c>
       <c r="H28" t="s">
-        <v>206</v>
-      </c>
-      <c r="I28" t="s">
-        <v>232</v>
+        <v>216</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2430,10 +1881,10 @@
         <v>1823.75</v>
       </c>
       <c r="H29" t="s">
-        <v>206</v>
-      </c>
-      <c r="I29" t="s">
-        <v>233</v>
+        <v>205</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2459,10 +1910,10 @@
         <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>206</v>
-      </c>
-      <c r="I30" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2488,10 +1939,10 @@
         <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>206</v>
-      </c>
-      <c r="I31" t="s">
-        <v>235</v>
+        <v>216</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2517,10 +1968,10 @@
         <v>10.56</v>
       </c>
       <c r="H32" t="s">
-        <v>206</v>
-      </c>
-      <c r="I32" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2546,10 +1997,10 @@
         <v>95</v>
       </c>
       <c r="H33" t="s">
-        <v>206</v>
-      </c>
-      <c r="I33" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2575,10 +2026,10 @@
         <v>43</v>
       </c>
       <c r="H34" t="s">
-        <v>206</v>
-      </c>
-      <c r="I34" t="s">
-        <v>237</v>
+        <v>216</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2604,10 +2055,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I35" t="s">
-        <v>238</v>
+        <v>216</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2633,10 +2084,10 @@
         <v>560</v>
       </c>
       <c r="H36" t="s">
-        <v>206</v>
-      </c>
-      <c r="I36" t="s">
-        <v>239</v>
+        <v>216</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2662,10 +2113,10 @@
         <v>410.76</v>
       </c>
       <c r="H37" t="s">
-        <v>206</v>
-      </c>
-      <c r="I37" t="s">
-        <v>240</v>
+        <v>217</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2691,10 +2142,10 @@
         <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>206</v>
-      </c>
-      <c r="I38" t="s">
-        <v>241</v>
+        <v>214</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2720,10 +2171,10 @@
         <v>10.99</v>
       </c>
       <c r="H39" t="s">
-        <v>206</v>
-      </c>
-      <c r="I39" t="s">
-        <v>241</v>
+        <v>214</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2749,10 +2200,10 @@
         <v>47</v>
       </c>
       <c r="H40" t="s">
-        <v>206</v>
-      </c>
-      <c r="I40" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2778,10 +2229,10 @@
         <v>2000</v>
       </c>
       <c r="H41" t="s">
-        <v>206</v>
-      </c>
-      <c r="I41" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2807,10 +2258,10 @@
         <v>24.89</v>
       </c>
       <c r="H42" t="s">
-        <v>206</v>
-      </c>
-      <c r="I42" t="s">
-        <v>242</v>
+        <v>216</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2836,10 +2287,10 @@
         <v>27.76</v>
       </c>
       <c r="H43" t="s">
-        <v>206</v>
-      </c>
-      <c r="I43" t="s">
-        <v>243</v>
+        <v>214</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2867,8 +2318,8 @@
       <c r="H44" t="s">
         <v>206</v>
       </c>
-      <c r="I44" t="s">
-        <v>210</v>
+      <c r="I44" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2894,10 +2345,10 @@
         <v>118.48</v>
       </c>
       <c r="H45" t="s">
-        <v>206</v>
-      </c>
-      <c r="I45" t="s">
-        <v>244</v>
+        <v>212</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2923,10 +2374,10 @@
         <v>120</v>
       </c>
       <c r="H46" t="s">
-        <v>206</v>
-      </c>
-      <c r="I46" t="s">
-        <v>245</v>
+        <v>208</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2952,10 +2403,10 @@
         <v>24.5</v>
       </c>
       <c r="H47" t="s">
-        <v>206</v>
-      </c>
-      <c r="I47" t="s">
-        <v>246</v>
+        <v>213</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2981,10 +2432,10 @@
         <v>88.48999999999999</v>
       </c>
       <c r="H48" t="s">
-        <v>206</v>
-      </c>
-      <c r="I48" t="s">
-        <v>247</v>
+        <v>209</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3010,10 +2461,10 @@
         <v>46.66</v>
       </c>
       <c r="H49" t="s">
-        <v>206</v>
-      </c>
-      <c r="I49" t="s">
-        <v>248</v>
+        <v>209</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3039,10 +2490,10 @@
         <v>71.7</v>
       </c>
       <c r="H50" t="s">
-        <v>206</v>
-      </c>
-      <c r="I50" t="s">
-        <v>249</v>
+        <v>207</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3068,10 +2519,10 @@
         <v>39</v>
       </c>
       <c r="H51" t="s">
-        <v>206</v>
-      </c>
-      <c r="I51" t="s">
-        <v>250</v>
+        <v>214</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3097,10 +2548,10 @@
         <v>1823.75</v>
       </c>
       <c r="H52" t="s">
-        <v>206</v>
-      </c>
-      <c r="I52" t="s">
-        <v>220</v>
+        <v>205</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3126,10 +2577,10 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>206</v>
-      </c>
-      <c r="I53" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3155,10 +2606,10 @@
         <v>45.81</v>
       </c>
       <c r="H54" t="s">
-        <v>206</v>
-      </c>
-      <c r="I54" t="s">
-        <v>251</v>
+        <v>209</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3184,10 +2635,10 @@
         <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>206</v>
-      </c>
-      <c r="I55" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3213,10 +2664,10 @@
         <v>47.47</v>
       </c>
       <c r="H56" t="s">
-        <v>206</v>
-      </c>
-      <c r="I56" t="s">
-        <v>252</v>
+        <v>214</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3242,10 +2693,10 @@
         <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>206</v>
-      </c>
-      <c r="I57" t="s">
-        <v>253</v>
+        <v>214</v>
+      </c>
+      <c r="I57" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -3271,10 +2722,10 @@
         <v>6</v>
       </c>
       <c r="H58" t="s">
-        <v>206</v>
-      </c>
-      <c r="I58" t="s">
-        <v>253</v>
+        <v>214</v>
+      </c>
+      <c r="I58" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3300,10 +2751,10 @@
         <v>590</v>
       </c>
       <c r="H59" t="s">
-        <v>206</v>
-      </c>
-      <c r="I59" t="s">
-        <v>254</v>
+        <v>214</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3329,10 +2780,10 @@
         <v>98.5</v>
       </c>
       <c r="H60" t="s">
-        <v>206</v>
-      </c>
-      <c r="I60" t="s">
-        <v>255</v>
+        <v>212</v>
+      </c>
+      <c r="I60" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3358,10 +2809,10 @@
         <v>14</v>
       </c>
       <c r="H61" t="s">
-        <v>206</v>
-      </c>
-      <c r="I61" t="s">
-        <v>256</v>
+        <v>214</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3387,10 +2838,10 @@
         <v>33.59</v>
       </c>
       <c r="H62" t="s">
-        <v>206</v>
-      </c>
-      <c r="I62" t="s">
-        <v>252</v>
+        <v>214</v>
+      </c>
+      <c r="I62" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3416,10 +2867,10 @@
         <v>29.9</v>
       </c>
       <c r="H63" t="s">
-        <v>206</v>
-      </c>
-      <c r="I63" t="s">
-        <v>257</v>
+        <v>214</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3445,10 +2896,10 @@
         <v>55</v>
       </c>
       <c r="H64" t="s">
-        <v>206</v>
-      </c>
-      <c r="I64" t="s">
-        <v>258</v>
+        <v>214</v>
+      </c>
+      <c r="I64" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3474,10 +2925,10 @@
         <v>66</v>
       </c>
       <c r="H65" t="s">
-        <v>206</v>
-      </c>
-      <c r="I65" t="s">
-        <v>259</v>
+        <v>214</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3503,10 +2954,10 @@
         <v>55</v>
       </c>
       <c r="H66" t="s">
-        <v>206</v>
-      </c>
-      <c r="I66" t="s">
-        <v>260</v>
+        <v>214</v>
+      </c>
+      <c r="I66" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3532,10 +2983,10 @@
         <v>55</v>
       </c>
       <c r="H67" t="s">
-        <v>206</v>
-      </c>
-      <c r="I67" t="s">
-        <v>261</v>
+        <v>214</v>
+      </c>
+      <c r="I67" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3561,10 +3012,10 @@
         <v>58.9</v>
       </c>
       <c r="H68" t="s">
-        <v>206</v>
-      </c>
-      <c r="I68" t="s">
-        <v>262</v>
+        <v>214</v>
+      </c>
+      <c r="I68" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3590,10 +3041,10 @@
         <v>-66</v>
       </c>
       <c r="H69" t="s">
-        <v>206</v>
-      </c>
-      <c r="I69" t="s">
-        <v>263</v>
+        <v>214</v>
+      </c>
+      <c r="I69" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3619,10 +3070,10 @@
         <v>7.99</v>
       </c>
       <c r="H70" t="s">
-        <v>206</v>
-      </c>
-      <c r="I70" t="s">
-        <v>227</v>
+        <v>214</v>
+      </c>
+      <c r="I70" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3648,10 +3099,10 @@
         <v>28.53</v>
       </c>
       <c r="H71" t="s">
-        <v>206</v>
-      </c>
-      <c r="I71" t="s">
-        <v>264</v>
+        <v>214</v>
+      </c>
+      <c r="I71" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3677,10 +3128,10 @@
         <v>20.9</v>
       </c>
       <c r="H72" t="s">
-        <v>206</v>
-      </c>
-      <c r="I72" t="s">
-        <v>265</v>
+        <v>215</v>
+      </c>
+      <c r="I72" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3706,10 +3157,10 @@
         <v>57</v>
       </c>
       <c r="H73" t="s">
-        <v>206</v>
-      </c>
-      <c r="I73" t="s">
-        <v>266</v>
+        <v>214</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3735,10 +3186,10 @@
         <v>18</v>
       </c>
       <c r="H74" t="s">
-        <v>206</v>
-      </c>
-      <c r="I74" t="s">
-        <v>267</v>
+        <v>214</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3764,10 +3215,10 @@
         <v>120</v>
       </c>
       <c r="H75" t="s">
-        <v>206</v>
-      </c>
-      <c r="I75" t="s">
-        <v>261</v>
+        <v>214</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3793,10 +3244,10 @@
         <v>17.45</v>
       </c>
       <c r="H76" t="s">
-        <v>206</v>
-      </c>
-      <c r="I76" t="s">
-        <v>268</v>
+        <v>214</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3822,10 +3273,10 @@
         <v>15.95</v>
       </c>
       <c r="H77" t="s">
-        <v>206</v>
-      </c>
-      <c r="I77" t="s">
-        <v>269</v>
+        <v>214</v>
+      </c>
+      <c r="I77" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3851,10 +3302,10 @@
         <v>42.82</v>
       </c>
       <c r="H78" t="s">
-        <v>206</v>
-      </c>
-      <c r="I78" t="s">
-        <v>232</v>
+        <v>216</v>
+      </c>
+      <c r="I78" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3880,10 +3331,10 @@
         <v>3000</v>
       </c>
       <c r="H79" t="s">
-        <v>206</v>
-      </c>
-      <c r="I79" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I79" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3909,10 +3360,10 @@
         <v>5000</v>
       </c>
       <c r="H80" t="s">
-        <v>206</v>
-      </c>
-      <c r="I80" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I80" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3938,10 +3389,10 @@
         <v>900</v>
       </c>
       <c r="H81" t="s">
-        <v>206</v>
-      </c>
-      <c r="I81" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3967,10 +3418,10 @@
         <v>120</v>
       </c>
       <c r="H82" t="s">
-        <v>206</v>
-      </c>
-      <c r="I82" t="s">
-        <v>270</v>
+        <v>205</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3996,10 +3447,10 @@
         <v>45.9</v>
       </c>
       <c r="H83" t="s">
-        <v>206</v>
-      </c>
-      <c r="I83" t="s">
-        <v>271</v>
+        <v>214</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -4025,10 +3476,10 @@
         <v>40</v>
       </c>
       <c r="H84" t="s">
-        <v>206</v>
-      </c>
-      <c r="I84" t="s">
-        <v>272</v>
+        <v>214</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -4054,10 +3505,10 @@
         <v>6997.09</v>
       </c>
       <c r="H85" t="s">
-        <v>206</v>
-      </c>
-      <c r="I85" t="s">
-        <v>273</v>
+        <v>214</v>
+      </c>
+      <c r="I85" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -4083,10 +3534,10 @@
         <v>811.35</v>
       </c>
       <c r="H86" t="s">
-        <v>206</v>
-      </c>
-      <c r="I86" t="s">
-        <v>274</v>
+        <v>216</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -4112,10 +3563,10 @@
         <v>71.5</v>
       </c>
       <c r="H87" t="s">
-        <v>206</v>
-      </c>
-      <c r="I87" t="s">
-        <v>275</v>
+        <v>216</v>
+      </c>
+      <c r="I87" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -4141,10 +3592,10 @@
         <v>1000</v>
       </c>
       <c r="H88" t="s">
-        <v>206</v>
-      </c>
-      <c r="I88" t="s">
-        <v>276</v>
+        <v>217</v>
+      </c>
+      <c r="I88" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4170,10 +3621,10 @@
         <v>1937.94</v>
       </c>
       <c r="H89" t="s">
-        <v>206</v>
-      </c>
-      <c r="I89" t="s">
-        <v>233</v>
+        <v>205</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -4199,10 +3650,10 @@
         <v>84.41</v>
       </c>
       <c r="H90" t="s">
-        <v>206</v>
-      </c>
-      <c r="I90" t="s">
-        <v>277</v>
+        <v>214</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -4228,10 +3679,10 @@
         <v>66</v>
       </c>
       <c r="H91" t="s">
-        <v>206</v>
-      </c>
-      <c r="I91" t="s">
-        <v>278</v>
+        <v>214</v>
+      </c>
+      <c r="I91" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -4257,10 +3708,10 @@
         <v>53</v>
       </c>
       <c r="H92" t="s">
-        <v>206</v>
-      </c>
-      <c r="I92" t="s">
-        <v>279</v>
+        <v>214</v>
+      </c>
+      <c r="I92" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -4286,10 +3737,10 @@
         <v>26</v>
       </c>
       <c r="H93" t="s">
-        <v>206</v>
-      </c>
-      <c r="I93" t="s">
-        <v>280</v>
+        <v>214</v>
+      </c>
+      <c r="I93" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -4315,10 +3766,10 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>206</v>
-      </c>
-      <c r="I94" t="s">
-        <v>281</v>
+        <v>214</v>
+      </c>
+      <c r="I94" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -4344,10 +3795,10 @@
         <v>500</v>
       </c>
       <c r="H95" t="s">
-        <v>206</v>
-      </c>
-      <c r="I95" t="s">
-        <v>276</v>
+        <v>217</v>
+      </c>
+      <c r="I95" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -4373,10 +3824,10 @@
         <v>17</v>
       </c>
       <c r="H96" t="s">
-        <v>206</v>
-      </c>
-      <c r="I96" t="s">
-        <v>282</v>
+        <v>214</v>
+      </c>
+      <c r="I96" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -4402,10 +3853,10 @@
         <v>8.5</v>
       </c>
       <c r="H97" t="s">
-        <v>206</v>
-      </c>
-      <c r="I97" t="s">
-        <v>283</v>
+        <v>214</v>
+      </c>
+      <c r="I97" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4431,10 +3882,10 @@
         <v>17</v>
       </c>
       <c r="H98" t="s">
-        <v>206</v>
-      </c>
-      <c r="I98" t="s">
-        <v>282</v>
+        <v>214</v>
+      </c>
+      <c r="I98" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4460,10 +3911,10 @@
         <v>25</v>
       </c>
       <c r="H99" t="s">
-        <v>206</v>
-      </c>
-      <c r="I99" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="I99" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4489,10 +3940,10 @@
         <v>115.08</v>
       </c>
       <c r="H100" t="s">
-        <v>206</v>
-      </c>
-      <c r="I100" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="I100" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4518,10 +3969,10 @@
         <v>29</v>
       </c>
       <c r="H101" t="s">
-        <v>206</v>
-      </c>
-      <c r="I101" t="s">
-        <v>284</v>
+        <v>214</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4547,10 +3998,10 @@
         <v>20</v>
       </c>
       <c r="H102" t="s">
-        <v>206</v>
-      </c>
-      <c r="I102" t="s">
-        <v>285</v>
+        <v>214</v>
+      </c>
+      <c r="I102" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4576,10 +4027,10 @@
         <v>80</v>
       </c>
       <c r="H103" t="s">
-        <v>206</v>
-      </c>
-      <c r="I103" t="s">
-        <v>286</v>
+        <v>214</v>
+      </c>
+      <c r="I103" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -4605,10 +4056,10 @@
         <v>31</v>
       </c>
       <c r="H104" t="s">
-        <v>206</v>
-      </c>
-      <c r="I104" t="s">
-        <v>287</v>
+        <v>214</v>
+      </c>
+      <c r="I104" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -4634,10 +4085,10 @@
         <v>25</v>
       </c>
       <c r="H105" t="s">
-        <v>206</v>
-      </c>
-      <c r="I105" t="s">
-        <v>288</v>
+        <v>214</v>
+      </c>
+      <c r="I105" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4663,10 +4114,10 @@
         <v>36</v>
       </c>
       <c r="H106" t="s">
-        <v>206</v>
-      </c>
-      <c r="I106" t="s">
-        <v>289</v>
+        <v>214</v>
+      </c>
+      <c r="I106" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4692,10 +4143,10 @@
         <v>10</v>
       </c>
       <c r="H107" t="s">
-        <v>206</v>
-      </c>
-      <c r="I107" t="s">
-        <v>290</v>
+        <v>214</v>
+      </c>
+      <c r="I107" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4721,10 +4172,10 @@
         <v>71</v>
       </c>
       <c r="H108" t="s">
-        <v>206</v>
-      </c>
-      <c r="I108" t="s">
-        <v>291</v>
+        <v>216</v>
+      </c>
+      <c r="I108" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4750,10 +4201,10 @@
         <v>30</v>
       </c>
       <c r="H109" t="s">
-        <v>206</v>
-      </c>
-      <c r="I109" t="s">
-        <v>292</v>
+        <v>214</v>
+      </c>
+      <c r="I109" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4779,10 +4230,10 @@
         <v>2000</v>
       </c>
       <c r="H110" t="s">
-        <v>206</v>
-      </c>
-      <c r="I110" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I110" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4808,10 +4259,10 @@
         <v>71.7</v>
       </c>
       <c r="H111" t="s">
-        <v>206</v>
-      </c>
-      <c r="I111" t="s">
-        <v>293</v>
+        <v>207</v>
+      </c>
+      <c r="I111" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4837,10 +4288,10 @@
         <v>98.5</v>
       </c>
       <c r="H112" t="s">
-        <v>206</v>
-      </c>
-      <c r="I112" t="s">
-        <v>294</v>
+        <v>212</v>
+      </c>
+      <c r="I112" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4866,10 +4317,10 @@
         <v>46.66</v>
       </c>
       <c r="H113" t="s">
-        <v>206</v>
-      </c>
-      <c r="I113" t="s">
-        <v>295</v>
+        <v>209</v>
+      </c>
+      <c r="I113" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4895,10 +4346,10 @@
         <v>115.71</v>
       </c>
       <c r="H114" t="s">
-        <v>206</v>
-      </c>
-      <c r="I114" t="s">
-        <v>296</v>
+        <v>214</v>
+      </c>
+      <c r="I114" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -4924,10 +4375,10 @@
         <v>120</v>
       </c>
       <c r="H115" t="s">
-        <v>206</v>
-      </c>
-      <c r="I115" t="s">
-        <v>297</v>
+        <v>208</v>
+      </c>
+      <c r="I115" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4953,10 +4404,10 @@
         <v>118.48</v>
       </c>
       <c r="H116" t="s">
-        <v>206</v>
-      </c>
-      <c r="I116" t="s">
-        <v>298</v>
+        <v>212</v>
+      </c>
+      <c r="I116" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -4982,10 +4433,10 @@
         <v>45.8</v>
       </c>
       <c r="H117" t="s">
-        <v>206</v>
-      </c>
-      <c r="I117" t="s">
-        <v>299</v>
+        <v>209</v>
+      </c>
+      <c r="I117" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -5011,10 +4462,10 @@
         <v>71</v>
       </c>
       <c r="H118" t="s">
-        <v>206</v>
-      </c>
-      <c r="I118" t="s">
-        <v>300</v>
+        <v>214</v>
+      </c>
+      <c r="I118" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -5040,10 +4491,10 @@
         <v>0</v>
       </c>
       <c r="H119" t="s">
-        <v>206</v>
-      </c>
-      <c r="I119" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I119" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -5069,10 +4520,10 @@
         <v>1937.94</v>
       </c>
       <c r="H120" t="s">
-        <v>206</v>
-      </c>
-      <c r="I120" t="s">
-        <v>220</v>
+        <v>205</v>
+      </c>
+      <c r="I120" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -5098,10 +4549,10 @@
         <v>0</v>
       </c>
       <c r="H121" t="s">
-        <v>206</v>
-      </c>
-      <c r="I121" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I121" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -5127,10 +4578,10 @@
         <v>112</v>
       </c>
       <c r="H122" t="s">
-        <v>206</v>
-      </c>
-      <c r="I122" t="s">
-        <v>301</v>
+        <v>214</v>
+      </c>
+      <c r="I122" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -5156,10 +4607,10 @@
         <v>89.90000000000001</v>
       </c>
       <c r="H123" t="s">
-        <v>206</v>
-      </c>
-      <c r="I123" t="s">
-        <v>302</v>
+        <v>208</v>
+      </c>
+      <c r="I123" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -5187,8 +4638,8 @@
       <c r="H124" t="s">
         <v>206</v>
       </c>
-      <c r="I124" t="s">
-        <v>303</v>
+      <c r="I124" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -5214,10 +4665,10 @@
         <v>12</v>
       </c>
       <c r="H125" t="s">
-        <v>206</v>
-      </c>
-      <c r="I125" t="s">
-        <v>253</v>
+        <v>214</v>
+      </c>
+      <c r="I125" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -5243,10 +4694,10 @@
         <v>6</v>
       </c>
       <c r="H126" t="s">
-        <v>206</v>
-      </c>
-      <c r="I126" t="s">
-        <v>253</v>
+        <v>214</v>
+      </c>
+      <c r="I126" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -5272,10 +4723,10 @@
         <v>14</v>
       </c>
       <c r="H127" t="s">
-        <v>206</v>
-      </c>
-      <c r="I127" t="s">
-        <v>304</v>
+        <v>214</v>
+      </c>
+      <c r="I127" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -5301,10 +4752,10 @@
         <v>60</v>
       </c>
       <c r="H128" t="s">
-        <v>206</v>
-      </c>
-      <c r="I128" t="s">
-        <v>305</v>
+        <v>214</v>
+      </c>
+      <c r="I128" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -5330,10 +4781,10 @@
         <v>113.93</v>
       </c>
       <c r="H129" t="s">
-        <v>206</v>
-      </c>
-      <c r="I129" t="s">
-        <v>306</v>
+        <v>214</v>
+      </c>
+      <c r="I129" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -5359,10 +4810,10 @@
         <v>79.90000000000001</v>
       </c>
       <c r="H130" t="s">
-        <v>206</v>
-      </c>
-      <c r="I130" t="s">
-        <v>307</v>
+        <v>214</v>
+      </c>
+      <c r="I130" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -5388,10 +4839,10 @@
         <v>29</v>
       </c>
       <c r="H131" t="s">
-        <v>206</v>
-      </c>
-      <c r="I131" t="s">
-        <v>308</v>
+        <v>214</v>
+      </c>
+      <c r="I131" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -5417,10 +4868,10 @@
         <v>15</v>
       </c>
       <c r="H132" t="s">
-        <v>206</v>
-      </c>
-      <c r="I132" t="s">
-        <v>309</v>
+        <v>214</v>
+      </c>
+      <c r="I132" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -5446,10 +4897,10 @@
         <v>20.9</v>
       </c>
       <c r="H133" t="s">
-        <v>206</v>
-      </c>
-      <c r="I133" t="s">
-        <v>265</v>
+        <v>215</v>
+      </c>
+      <c r="I133" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -5475,10 +4926,10 @@
         <v>149</v>
       </c>
       <c r="H134" t="s">
-        <v>206</v>
-      </c>
-      <c r="I134" t="s">
-        <v>310</v>
+        <v>214</v>
+      </c>
+      <c r="I134" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -5504,10 +4955,10 @@
         <v>55</v>
       </c>
       <c r="H135" t="s">
-        <v>206</v>
-      </c>
-      <c r="I135" t="s">
-        <v>311</v>
+        <v>214</v>
+      </c>
+      <c r="I135" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -5535,8 +4986,8 @@
       <c r="H136" t="s">
         <v>206</v>
       </c>
-      <c r="I136" t="s">
-        <v>312</v>
+      <c r="I136" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -5562,10 +5013,10 @@
         <v>45</v>
       </c>
       <c r="H137" t="s">
-        <v>206</v>
-      </c>
-      <c r="I137" t="s">
-        <v>313</v>
+        <v>214</v>
+      </c>
+      <c r="I137" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -5593,8 +5044,8 @@
       <c r="H138" t="s">
         <v>206</v>
       </c>
-      <c r="I138" t="s">
-        <v>314</v>
+      <c r="I138" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -5620,10 +5071,10 @@
         <v>17.45</v>
       </c>
       <c r="H139" t="s">
-        <v>206</v>
-      </c>
-      <c r="I139" t="s">
-        <v>268</v>
+        <v>214</v>
+      </c>
+      <c r="I139" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -5649,10 +5100,10 @@
         <v>2000</v>
       </c>
       <c r="H140" t="s">
-        <v>206</v>
-      </c>
-      <c r="I140" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I140" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -5678,10 +5129,10 @@
         <v>34</v>
       </c>
       <c r="H141" t="s">
-        <v>206</v>
-      </c>
-      <c r="I141" t="s">
-        <v>315</v>
+        <v>214</v>
+      </c>
+      <c r="I141" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -5707,10 +5158,10 @@
         <v>40</v>
       </c>
       <c r="H142" t="s">
-        <v>206</v>
-      </c>
-      <c r="I142" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="I142" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -5736,10 +5187,10 @@
         <v>40</v>
       </c>
       <c r="H143" t="s">
-        <v>206</v>
-      </c>
-      <c r="I143" t="s">
-        <v>316</v>
+        <v>214</v>
+      </c>
+      <c r="I143" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -5765,10 +5216,10 @@
         <v>37.73</v>
       </c>
       <c r="H144" t="s">
-        <v>206</v>
-      </c>
-      <c r="I144" t="s">
-        <v>317</v>
+        <v>214</v>
+      </c>
+      <c r="I144" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -5794,10 +5245,10 @@
         <v>37.78</v>
       </c>
       <c r="H145" t="s">
-        <v>206</v>
-      </c>
-      <c r="I145" t="s">
-        <v>318</v>
+        <v>214</v>
+      </c>
+      <c r="I145" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -5823,10 +5274,10 @@
         <v>39.9</v>
       </c>
       <c r="H146" t="s">
-        <v>206</v>
-      </c>
-      <c r="I146" t="s">
-        <v>319</v>
+        <v>214</v>
+      </c>
+      <c r="I146" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -5852,10 +5303,10 @@
         <v>46</v>
       </c>
       <c r="H147" t="s">
-        <v>206</v>
-      </c>
-      <c r="I147" t="s">
-        <v>320</v>
+        <v>214</v>
+      </c>
+      <c r="I147" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -5881,10 +5332,10 @@
         <v>50</v>
       </c>
       <c r="H148" t="s">
-        <v>206</v>
-      </c>
-      <c r="I148" t="s">
-        <v>321</v>
+        <v>216</v>
+      </c>
+      <c r="I148" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -5910,10 +5361,10 @@
         <v>1837.54</v>
       </c>
       <c r="H149" t="s">
-        <v>206</v>
-      </c>
-      <c r="I149" t="s">
-        <v>233</v>
+        <v>205</v>
+      </c>
+      <c r="I149" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5939,10 +5390,10 @@
         <v>19.5</v>
       </c>
       <c r="H150" t="s">
-        <v>206</v>
-      </c>
-      <c r="I150" t="s">
-        <v>285</v>
+        <v>214</v>
+      </c>
+      <c r="I150" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5968,10 +5419,10 @@
         <v>1400</v>
       </c>
       <c r="H151" t="s">
-        <v>206</v>
-      </c>
-      <c r="I151" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I151" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5997,10 +5448,10 @@
         <v>632</v>
       </c>
       <c r="H152" t="s">
-        <v>206</v>
-      </c>
-      <c r="I152" t="s">
-        <v>274</v>
+        <v>216</v>
+      </c>
+      <c r="I152" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -6026,10 +5477,10 @@
         <v>1372.93</v>
       </c>
       <c r="H153" t="s">
-        <v>206</v>
-      </c>
-      <c r="I153" t="s">
-        <v>322</v>
+        <v>214</v>
+      </c>
+      <c r="I153" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -6055,10 +5506,10 @@
         <v>1372.93</v>
       </c>
       <c r="H154" t="s">
-        <v>206</v>
-      </c>
-      <c r="I154" t="s">
-        <v>322</v>
+        <v>214</v>
+      </c>
+      <c r="I154" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -6084,10 +5535,10 @@
         <v>38</v>
       </c>
       <c r="H155" t="s">
-        <v>206</v>
-      </c>
-      <c r="I155" t="s">
-        <v>323</v>
+        <v>214</v>
+      </c>
+      <c r="I155" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -6113,10 +5564,10 @@
         <v>18</v>
       </c>
       <c r="H156" t="s">
-        <v>206</v>
-      </c>
-      <c r="I156" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I156" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -6142,10 +5593,10 @@
         <v>45.5</v>
       </c>
       <c r="H157" t="s">
-        <v>206</v>
-      </c>
-      <c r="I157" t="s">
-        <v>325</v>
+        <v>214</v>
+      </c>
+      <c r="I157" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -6171,10 +5622,10 @@
         <v>50</v>
       </c>
       <c r="H158" t="s">
-        <v>206</v>
-      </c>
-      <c r="I158" t="s">
-        <v>326</v>
+        <v>214</v>
+      </c>
+      <c r="I158" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -6200,10 +5651,10 @@
         <v>57</v>
       </c>
       <c r="H159" t="s">
-        <v>206</v>
-      </c>
-      <c r="I159" t="s">
-        <v>327</v>
+        <v>214</v>
+      </c>
+      <c r="I159" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -6229,10 +5680,10 @@
         <v>8</v>
       </c>
       <c r="H160" t="s">
-        <v>206</v>
-      </c>
-      <c r="I160" t="s">
-        <v>328</v>
+        <v>214</v>
+      </c>
+      <c r="I160" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -6258,10 +5709,10 @@
         <v>18</v>
       </c>
       <c r="H161" t="s">
-        <v>206</v>
-      </c>
-      <c r="I161" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I161" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -6287,10 +5738,10 @@
         <v>39</v>
       </c>
       <c r="H162" t="s">
-        <v>206</v>
-      </c>
-      <c r="I162" t="s">
-        <v>329</v>
+        <v>214</v>
+      </c>
+      <c r="I162" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -6316,10 +5767,10 @@
         <v>15</v>
       </c>
       <c r="H163" t="s">
-        <v>206</v>
-      </c>
-      <c r="I163" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I163" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -6345,10 +5796,10 @@
         <v>15</v>
       </c>
       <c r="H164" t="s">
-        <v>206</v>
-      </c>
-      <c r="I164" t="s">
-        <v>330</v>
+        <v>214</v>
+      </c>
+      <c r="I164" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -6374,10 +5825,10 @@
         <v>23</v>
       </c>
       <c r="H165" t="s">
-        <v>206</v>
-      </c>
-      <c r="I165" t="s">
-        <v>331</v>
+        <v>214</v>
+      </c>
+      <c r="I165" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -6403,10 +5854,10 @@
         <v>76.48999999999999</v>
       </c>
       <c r="H166" t="s">
-        <v>206</v>
-      </c>
-      <c r="I166" t="s">
-        <v>332</v>
+        <v>216</v>
+      </c>
+      <c r="I166" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -6432,10 +5883,10 @@
         <v>12</v>
       </c>
       <c r="H167" t="s">
-        <v>206</v>
-      </c>
-      <c r="I167" t="s">
-        <v>328</v>
+        <v>214</v>
+      </c>
+      <c r="I167" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -6461,10 +5912,10 @@
         <v>28</v>
       </c>
       <c r="H168" t="s">
-        <v>206</v>
-      </c>
-      <c r="I168" t="s">
-        <v>333</v>
+        <v>214</v>
+      </c>
+      <c r="I168" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -6490,10 +5941,10 @@
         <v>15</v>
       </c>
       <c r="H169" t="s">
-        <v>206</v>
-      </c>
-      <c r="I169" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I169" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -6519,10 +5970,10 @@
         <v>15</v>
       </c>
       <c r="H170" t="s">
-        <v>206</v>
-      </c>
-      <c r="I170" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I170" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -6548,10 +5999,10 @@
         <v>15</v>
       </c>
       <c r="H171" t="s">
-        <v>206</v>
-      </c>
-      <c r="I171" t="s">
-        <v>334</v>
+        <v>214</v>
+      </c>
+      <c r="I171" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -6577,10 +6028,10 @@
         <v>15</v>
       </c>
       <c r="H172" t="s">
-        <v>206</v>
-      </c>
-      <c r="I172" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I172" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -6606,10 +6057,10 @@
         <v>10</v>
       </c>
       <c r="H173" t="s">
-        <v>206</v>
-      </c>
-      <c r="I173" t="s">
-        <v>291</v>
+        <v>216</v>
+      </c>
+      <c r="I173" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -6635,10 +6086,10 @@
         <v>5.25</v>
       </c>
       <c r="H174" t="s">
-        <v>206</v>
-      </c>
-      <c r="I174" t="s">
-        <v>335</v>
+        <v>214</v>
+      </c>
+      <c r="I174" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -6664,10 +6115,10 @@
         <v>10.59</v>
       </c>
       <c r="H175" t="s">
-        <v>206</v>
-      </c>
-      <c r="I175" t="s">
-        <v>336</v>
+        <v>214</v>
+      </c>
+      <c r="I175" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -6693,10 +6144,10 @@
         <v>68.77</v>
       </c>
       <c r="H176" t="s">
-        <v>206</v>
-      </c>
-      <c r="I176" t="s">
-        <v>337</v>
+        <v>214</v>
+      </c>
+      <c r="I176" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -6722,10 +6173,10 @@
         <v>31.9</v>
       </c>
       <c r="H177" t="s">
-        <v>206</v>
-      </c>
-      <c r="I177" t="s">
-        <v>338</v>
+        <v>214</v>
+      </c>
+      <c r="I177" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -6751,10 +6202,10 @@
         <v>162</v>
       </c>
       <c r="H178" t="s">
-        <v>206</v>
-      </c>
-      <c r="I178" t="s">
-        <v>339</v>
+        <v>214</v>
+      </c>
+      <c r="I178" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -6780,10 +6231,10 @@
         <v>60.7</v>
       </c>
       <c r="H179" t="s">
-        <v>206</v>
-      </c>
-      <c r="I179" t="s">
-        <v>340</v>
+        <v>214</v>
+      </c>
+      <c r="I179" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -6809,10 +6260,10 @@
         <v>30</v>
       </c>
       <c r="H180" t="s">
-        <v>206</v>
-      </c>
-      <c r="I180" t="s">
-        <v>341</v>
+        <v>214</v>
+      </c>
+      <c r="I180" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -6838,10 +6289,10 @@
         <v>3000</v>
       </c>
       <c r="H181" t="s">
-        <v>206</v>
-      </c>
-      <c r="I181" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I181" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -6867,10 +6318,10 @@
         <v>20</v>
       </c>
       <c r="H182" t="s">
-        <v>206</v>
-      </c>
-      <c r="I182" t="s">
-        <v>342</v>
+        <v>214</v>
+      </c>
+      <c r="I182" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -6896,10 +6347,10 @@
         <v>22</v>
       </c>
       <c r="H183" t="s">
-        <v>206</v>
-      </c>
-      <c r="I183" t="s">
-        <v>342</v>
+        <v>214</v>
+      </c>
+      <c r="I183" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -6925,10 +6376,10 @@
         <v>30</v>
       </c>
       <c r="H184" t="s">
-        <v>206</v>
-      </c>
-      <c r="I184" t="s">
-        <v>342</v>
+        <v>214</v>
+      </c>
+      <c r="I184" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -6956,8 +6407,8 @@
       <c r="H185" t="s">
         <v>206</v>
       </c>
-      <c r="I185" t="s">
-        <v>343</v>
+      <c r="I185" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -6983,10 +6434,10 @@
         <v>120</v>
       </c>
       <c r="H186" t="s">
-        <v>206</v>
-      </c>
-      <c r="I186" t="s">
-        <v>344</v>
+        <v>208</v>
+      </c>
+      <c r="I186" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -7012,10 +6463,10 @@
         <v>71.7</v>
       </c>
       <c r="H187" t="s">
-        <v>206</v>
-      </c>
-      <c r="I187" t="s">
-        <v>345</v>
+        <v>207</v>
+      </c>
+      <c r="I187" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -7043,8 +6494,8 @@
       <c r="H188" t="s">
         <v>206</v>
       </c>
-      <c r="I188" t="s">
-        <v>346</v>
+      <c r="I188" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -7072,8 +6523,8 @@
       <c r="H189" t="s">
         <v>206</v>
       </c>
-      <c r="I189" t="s">
-        <v>347</v>
+      <c r="I189" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -7099,10 +6550,10 @@
         <v>73.92</v>
       </c>
       <c r="H190" t="s">
-        <v>206</v>
-      </c>
-      <c r="I190" t="s">
-        <v>348</v>
+        <v>209</v>
+      </c>
+      <c r="I190" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -7128,10 +6579,10 @@
         <v>14.97</v>
       </c>
       <c r="H191" t="s">
-        <v>206</v>
-      </c>
-      <c r="I191" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I191" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -7157,10 +6608,10 @@
         <v>0</v>
       </c>
       <c r="H192" t="s">
-        <v>206</v>
-      </c>
-      <c r="I192" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I192" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -7186,10 +6637,10 @@
         <v>0</v>
       </c>
       <c r="H193" t="s">
-        <v>206</v>
-      </c>
-      <c r="I193" t="s">
-        <v>225</v>
+        <v>208</v>
+      </c>
+      <c r="I193" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -7215,10 +6666,10 @@
         <v>1837.54</v>
       </c>
       <c r="H194" t="s">
-        <v>206</v>
-      </c>
-      <c r="I194" t="s">
-        <v>220</v>
+        <v>205</v>
+      </c>
+      <c r="I194" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -7244,10 +6695,10 @@
         <v>59</v>
       </c>
       <c r="H195" t="s">
-        <v>206</v>
-      </c>
-      <c r="I195" t="s">
-        <v>350</v>
+        <v>214</v>
+      </c>
+      <c r="I195" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -7273,10 +6724,10 @@
         <v>9.99</v>
       </c>
       <c r="H196" t="s">
-        <v>206</v>
-      </c>
-      <c r="I196" t="s">
-        <v>351</v>
+        <v>214</v>
+      </c>
+      <c r="I196" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -7302,10 +6753,10 @@
         <v>30</v>
       </c>
       <c r="H197" t="s">
-        <v>206</v>
-      </c>
-      <c r="I197" t="s">
-        <v>352</v>
+        <v>214</v>
+      </c>
+      <c r="I197" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -7331,10 +6782,10 @@
         <v>46.89</v>
       </c>
       <c r="H198" t="s">
-        <v>206</v>
-      </c>
-      <c r="I198" t="s">
-        <v>353</v>
+        <v>214</v>
+      </c>
+      <c r="I198" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -7360,10 +6811,10 @@
         <v>18.11</v>
       </c>
       <c r="H199" t="s">
-        <v>206</v>
-      </c>
-      <c r="I199" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I199" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -7389,10 +6840,10 @@
         <v>14.98</v>
       </c>
       <c r="H200" t="s">
-        <v>206</v>
-      </c>
-      <c r="I200" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I200" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -7418,10 +6869,10 @@
         <v>52.58</v>
       </c>
       <c r="H201" t="s">
-        <v>206</v>
-      </c>
-      <c r="I201" t="s">
-        <v>354</v>
+        <v>214</v>
+      </c>
+      <c r="I201" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -7447,10 +6898,10 @@
         <v>19.98</v>
       </c>
       <c r="H202" t="s">
-        <v>206</v>
-      </c>
-      <c r="I202" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I202" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -7476,10 +6927,10 @@
         <v>11.9</v>
       </c>
       <c r="H203" t="s">
-        <v>206</v>
-      </c>
-      <c r="I203" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I203" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -7505,10 +6956,10 @@
         <v>27.98</v>
       </c>
       <c r="H204" t="s">
-        <v>206</v>
-      </c>
-      <c r="I204" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I204" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -7536,8 +6987,8 @@
       <c r="H205" t="s">
         <v>206</v>
       </c>
-      <c r="I205" t="s">
-        <v>355</v>
+      <c r="I205" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -7563,10 +7014,10 @@
         <v>150</v>
       </c>
       <c r="H206" t="s">
-        <v>206</v>
-      </c>
-      <c r="I206" t="s">
-        <v>356</v>
+        <v>214</v>
+      </c>
+      <c r="I206" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -7592,10 +7043,10 @@
         <v>28.94</v>
       </c>
       <c r="H207" t="s">
-        <v>206</v>
-      </c>
-      <c r="I207" t="s">
-        <v>349</v>
+        <v>214</v>
+      </c>
+      <c r="I207" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -7621,10 +7072,10 @@
         <v>20.9</v>
       </c>
       <c r="H208" t="s">
-        <v>206</v>
-      </c>
-      <c r="I208" t="s">
-        <v>357</v>
+        <v>215</v>
+      </c>
+      <c r="I208" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -7650,10 +7101,10 @@
         <v>93.84999999999999</v>
       </c>
       <c r="H209" t="s">
-        <v>206</v>
-      </c>
-      <c r="I209" t="s">
-        <v>358</v>
+        <v>214</v>
+      </c>
+      <c r="I209" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -7679,10 +7130,10 @@
         <v>68.90000000000001</v>
       </c>
       <c r="H210" t="s">
-        <v>206</v>
-      </c>
-      <c r="I210" t="s">
-        <v>359</v>
+        <v>214</v>
+      </c>
+      <c r="I210" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -7708,10 +7159,10 @@
         <v>18.95</v>
       </c>
       <c r="H211" t="s">
-        <v>206</v>
-      </c>
-      <c r="I211" t="s">
-        <v>360</v>
+        <v>214</v>
+      </c>
+      <c r="I211" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -7737,10 +7188,10 @@
         <v>19.95</v>
       </c>
       <c r="H212" t="s">
-        <v>206</v>
-      </c>
-      <c r="I212" t="s">
-        <v>268</v>
+        <v>214</v>
+      </c>
+      <c r="I212" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -7766,10 +7217,10 @@
         <v>15</v>
       </c>
       <c r="H213" t="s">
-        <v>206</v>
-      </c>
-      <c r="I213" t="s">
-        <v>361</v>
+        <v>214</v>
+      </c>
+      <c r="I213" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -7795,10 +7246,10 @@
         <v>21.5</v>
       </c>
       <c r="H214" t="s">
-        <v>206</v>
-      </c>
-      <c r="I214" t="s">
-        <v>362</v>
+        <v>214</v>
+      </c>
+      <c r="I214" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -7824,10 +7275,10 @@
         <v>10</v>
       </c>
       <c r="H215" t="s">
-        <v>206</v>
-      </c>
-      <c r="I215" t="s">
-        <v>363</v>
+        <v>214</v>
+      </c>
+      <c r="I215" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -7853,10 +7304,10 @@
         <v>57</v>
       </c>
       <c r="H216" t="s">
-        <v>206</v>
-      </c>
-      <c r="I216" t="s">
-        <v>364</v>
+        <v>214</v>
+      </c>
+      <c r="I216" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -7882,10 +7333,10 @@
         <v>29</v>
       </c>
       <c r="H217" t="s">
-        <v>206</v>
-      </c>
-      <c r="I217" t="s">
-        <v>284</v>
+        <v>214</v>
+      </c>
+      <c r="I217" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -7911,10 +7362,10 @@
         <v>1517.33</v>
       </c>
       <c r="H218" t="s">
-        <v>206</v>
-      </c>
-      <c r="I218" t="s">
-        <v>240</v>
+        <v>217</v>
+      </c>
+      <c r="I218" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -7940,10 +7391,10 @@
         <v>120</v>
       </c>
       <c r="H219" t="s">
-        <v>206</v>
-      </c>
-      <c r="I219" t="s">
-        <v>365</v>
+        <v>216</v>
+      </c>
+      <c r="I219" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -7969,10 +7420,10 @@
         <v>5</v>
       </c>
       <c r="H220" t="s">
-        <v>206</v>
-      </c>
-      <c r="I220" t="s">
-        <v>366</v>
+        <v>214</v>
+      </c>
+      <c r="I220" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -7998,10 +7449,10 @@
         <v>10</v>
       </c>
       <c r="H221" t="s">
-        <v>206</v>
-      </c>
-      <c r="I221" t="s">
-        <v>367</v>
+        <v>214</v>
+      </c>
+      <c r="I221" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -8027,10 +7478,10 @@
         <v>33</v>
       </c>
       <c r="H222" t="s">
-        <v>206</v>
-      </c>
-      <c r="I222" t="s">
-        <v>239</v>
+        <v>216</v>
+      </c>
+      <c r="I222" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -8056,10 +7507,10 @@
         <v>34.2</v>
       </c>
       <c r="H223" t="s">
-        <v>206</v>
-      </c>
-      <c r="I223" t="s">
-        <v>368</v>
+        <v>214</v>
+      </c>
+      <c r="I223" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -8085,10 +7536,10 @@
         <v>29.4</v>
       </c>
       <c r="H224" t="s">
-        <v>206</v>
-      </c>
-      <c r="I224" t="s">
-        <v>369</v>
+        <v>214</v>
+      </c>
+      <c r="I224" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:9">
@@ -8114,10 +7565,10 @@
         <v>13.9</v>
       </c>
       <c r="H225" t="s">
-        <v>206</v>
-      </c>
-      <c r="I225" t="s">
-        <v>369</v>
+        <v>214</v>
+      </c>
+      <c r="I225" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -8143,10 +7594,10 @@
         <v>25.5</v>
       </c>
       <c r="H226" t="s">
-        <v>206</v>
-      </c>
-      <c r="I226" t="s">
-        <v>370</v>
+        <v>214</v>
+      </c>
+      <c r="I226" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -8172,10 +7623,10 @@
         <v>75.08</v>
       </c>
       <c r="H227" t="s">
-        <v>206</v>
-      </c>
-      <c r="I227" t="s">
-        <v>277</v>
+        <v>214</v>
+      </c>
+      <c r="I227" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -8201,10 +7652,10 @@
         <v>1434.02</v>
       </c>
       <c r="H228" t="s">
-        <v>206</v>
-      </c>
-      <c r="I228" t="s">
-        <v>233</v>
+        <v>205</v>
+      </c>
+      <c r="I228" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:9">
@@ -8230,10 +7681,10 @@
         <v>29</v>
       </c>
       <c r="H229" t="s">
-        <v>206</v>
-      </c>
-      <c r="I229" t="s">
-        <v>284</v>
+        <v>214</v>
+      </c>
+      <c r="I229" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -8259,10 +7710,10 @@
         <v>1000</v>
       </c>
       <c r="H230" t="s">
-        <v>206</v>
-      </c>
-      <c r="I230" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="I230" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -8288,10 +7739,10 @@
         <v>31</v>
       </c>
       <c r="H231" t="s">
-        <v>206</v>
-      </c>
-      <c r="I231" t="s">
-        <v>371</v>
+        <v>214</v>
+      </c>
+      <c r="I231" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -8317,10 +7768,10 @@
         <v>37.44</v>
       </c>
       <c r="H232" t="s">
-        <v>206</v>
-      </c>
-      <c r="I232" t="s">
-        <v>372</v>
+        <v>214</v>
+      </c>
+      <c r="I232" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:9">
@@ -8346,10 +7797,10 @@
         <v>20</v>
       </c>
       <c r="H233" t="s">
-        <v>206</v>
-      </c>
-      <c r="I233" t="s">
-        <v>373</v>
+        <v>216</v>
+      </c>
+      <c r="I233" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="234" spans="1:9">
@@ -8375,10 +7826,10 @@
         <v>56</v>
       </c>
       <c r="H234" t="s">
-        <v>206</v>
-      </c>
-      <c r="I234" t="s">
-        <v>374</v>
+        <v>214</v>
+      </c>
+      <c r="I234" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -8404,10 +7855,10 @@
         <v>86.72</v>
       </c>
       <c r="H235" t="s">
-        <v>206</v>
-      </c>
-      <c r="I235" t="s">
-        <v>375</v>
+        <v>214</v>
+      </c>
+      <c r="I235" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -8433,10 +7884,10 @@
         <v>17</v>
       </c>
       <c r="H236" t="s">
-        <v>206</v>
-      </c>
-      <c r="I236" t="s">
-        <v>376</v>
+        <v>214</v>
+      </c>
+      <c r="I236" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -8462,10 +7913,10 @@
         <v>5</v>
       </c>
       <c r="H237" t="s">
-        <v>206</v>
-      </c>
-      <c r="I237" t="s">
-        <v>377</v>
+        <v>214</v>
+      </c>
+      <c r="I237" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -8491,10 +7942,10 @@
         <v>12</v>
       </c>
       <c r="H238" t="s">
-        <v>206</v>
-      </c>
-      <c r="I238" t="s">
-        <v>378</v>
+        <v>214</v>
+      </c>
+      <c r="I238" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -8520,10 +7971,10 @@
         <v>195</v>
       </c>
       <c r="H239" t="s">
-        <v>206</v>
-      </c>
-      <c r="I239" t="s">
-        <v>379</v>
+        <v>216</v>
+      </c>
+      <c r="I239" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -8549,10 +8000,10 @@
         <v>10</v>
       </c>
       <c r="H240" t="s">
-        <v>206</v>
-      </c>
-      <c r="I240" t="s">
-        <v>380</v>
+        <v>214</v>
+      </c>
+      <c r="I240" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -8578,10 +8029,10 @@
         <v>15</v>
       </c>
       <c r="H241" t="s">
-        <v>206</v>
-      </c>
-      <c r="I241" t="s">
-        <v>381</v>
+        <v>214</v>
+      </c>
+      <c r="I241" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -8607,10 +8058,10 @@
         <v>19.99</v>
       </c>
       <c r="H242" t="s">
-        <v>206</v>
-      </c>
-      <c r="I242" t="s">
-        <v>382</v>
+        <v>214</v>
+      </c>
+      <c r="I242" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:9">
@@ -8636,10 +8087,10 @@
         <v>10</v>
       </c>
       <c r="H243" t="s">
-        <v>206</v>
-      </c>
-      <c r="I243" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="I243" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -8665,10 +8116,10 @@
         <v>1</v>
       </c>
       <c r="H244" t="s">
-        <v>206</v>
-      </c>
-      <c r="I244" t="s">
-        <v>383</v>
+        <v>216</v>
+      </c>
+      <c r="I244" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -8694,10 +8145,10 @@
         <v>200</v>
       </c>
       <c r="H245" t="s">
-        <v>206</v>
-      </c>
-      <c r="I245" t="s">
-        <v>384</v>
+        <v>214</v>
+      </c>
+      <c r="I245" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -8723,10 +8174,10 @@
         <v>37.43</v>
       </c>
       <c r="H246" t="s">
-        <v>206</v>
-      </c>
-      <c r="I246" t="s">
-        <v>385</v>
+        <v>216</v>
+      </c>
+      <c r="I246" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -8752,10 +8203,10 @@
         <v>20</v>
       </c>
       <c r="H247" t="s">
-        <v>206</v>
-      </c>
-      <c r="I247" t="s">
-        <v>386</v>
+        <v>216</v>
+      </c>
+      <c r="I247" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -8781,10 +8232,10 @@
         <v>61</v>
       </c>
       <c r="H248" t="s">
-        <v>206</v>
-      </c>
-      <c r="I248" t="s">
-        <v>387</v>
+        <v>216</v>
+      </c>
+      <c r="I248" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -8810,10 +8261,10 @@
         <v>75</v>
       </c>
       <c r="H249" t="s">
-        <v>206</v>
-      </c>
-      <c r="I249" t="s">
-        <v>388</v>
+        <v>216</v>
+      </c>
+      <c r="I249" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -8839,10 +8290,10 @@
         <v>47</v>
       </c>
       <c r="H250" t="s">
-        <v>206</v>
-      </c>
-      <c r="I250" t="s">
-        <v>327</v>
+        <v>214</v>
+      </c>
+      <c r="I250" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:9">
@@ -8868,10 +8319,10 @@
         <v>30</v>
       </c>
       <c r="H251" t="s">
-        <v>206</v>
-      </c>
-      <c r="I251" t="s">
-        <v>389</v>
+        <v>214</v>
+      </c>
+      <c r="I251" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -8897,10 +8348,10 @@
         <v>35</v>
       </c>
       <c r="H252" t="s">
-        <v>206</v>
-      </c>
-      <c r="I252" t="s">
-        <v>390</v>
+        <v>214</v>
+      </c>
+      <c r="I252" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -8926,10 +8377,10 @@
         <v>54.9</v>
       </c>
       <c r="H253" t="s">
-        <v>206</v>
-      </c>
-      <c r="I253" t="s">
-        <v>391</v>
+        <v>214</v>
+      </c>
+      <c r="I253" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="254" spans="1:9">
@@ -8955,10 +8406,10 @@
         <v>154.97</v>
       </c>
       <c r="H254" t="s">
-        <v>206</v>
-      </c>
-      <c r="I254" t="s">
-        <v>392</v>
+        <v>214</v>
+      </c>
+      <c r="I254" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="255" spans="1:9">
@@ -8984,10 +8435,10 @@
         <v>120.9</v>
       </c>
       <c r="H255" t="s">
-        <v>206</v>
-      </c>
-      <c r="I255" t="s">
-        <v>384</v>
+        <v>214</v>
+      </c>
+      <c r="I255" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="256" spans="1:9">
@@ -9013,10 +8464,10 @@
         <v>34.9</v>
       </c>
       <c r="H256" t="s">
-        <v>206</v>
-      </c>
-      <c r="I256" t="s">
-        <v>393</v>
+        <v>216</v>
+      </c>
+      <c r="I256" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:9">
@@ -9042,10 +8493,10 @@
         <v>70</v>
       </c>
       <c r="H257" t="s">
-        <v>206</v>
-      </c>
-      <c r="I257" t="s">
-        <v>394</v>
+        <v>216</v>
+      </c>
+      <c r="I257" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:9">
@@ -9071,10 +8522,10 @@
         <v>12</v>
       </c>
       <c r="H258" t="s">
-        <v>206</v>
-      </c>
-      <c r="I258" t="s">
-        <v>324</v>
+        <v>214</v>
+      </c>
+      <c r="I258" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="259" spans="1:9">
@@ -9100,10 +8551,10 @@
         <v>28.4</v>
       </c>
       <c r="H259" t="s">
-        <v>206</v>
-      </c>
-      <c r="I259" t="s">
-        <v>395</v>
+        <v>214</v>
+      </c>
+      <c r="I259" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:9">
@@ -9129,10 +8580,10 @@
         <v>60</v>
       </c>
       <c r="H260" t="s">
-        <v>206</v>
-      </c>
-      <c r="I260" t="s">
-        <v>396</v>
+        <v>214</v>
+      </c>
+      <c r="I260" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="261" spans="1:9">
@@ -9158,10 +8609,10 @@
         <v>68.92</v>
       </c>
       <c r="H261" t="s">
-        <v>206</v>
-      </c>
-      <c r="I261" t="s">
-        <v>397</v>
+        <v>214</v>
+      </c>
+      <c r="I261" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="262" spans="1:9">
@@ -9187,10 +8638,10 @@
         <v>12.5</v>
       </c>
       <c r="H262" t="s">
-        <v>206</v>
-      </c>
-      <c r="I262" t="s">
-        <v>398</v>
+        <v>214</v>
+      </c>
+      <c r="I262" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -9216,10 +8667,10 @@
         <v>10</v>
       </c>
       <c r="H263" t="s">
-        <v>206</v>
-      </c>
-      <c r="I263" t="s">
-        <v>399</v>
+        <v>214</v>
+      </c>
+      <c r="I263" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -9245,10 +8696,10 @@
         <v>99.90000000000001</v>
       </c>
       <c r="H264" t="s">
-        <v>206</v>
-      </c>
-      <c r="I264" t="s">
-        <v>400</v>
+        <v>216</v>
+      </c>
+      <c r="I264" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9258,7 +8709,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9272,31 +8723,31 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>401</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B2">
-        <v>259</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -9304,6 +8755,78 @@
         <v>208</v>
       </c>
       <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
     </row>
@@ -9337,7 +8860,7 @@
         <v>205</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>402</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>